<commit_message>
add final review checklist
</commit_message>
<xml_diff>
--- a/project/templates/Review Checklist for  Functional Test.xlsx
+++ b/project/templates/Review Checklist for  Functional Test.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="55">
   <si>
     <t>TESTCASE REVIEW CHECKLIST</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Does the test case document include document name, version, and release date?</t>
+  </si>
+  <si>
+    <t>✔</t>
   </si>
   <si>
     <t>Mandatory</t>
@@ -201,7 +204,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +243,12 @@
       <sz val="14"/>
       <color rgb="FF156082"/>
       <name val="Aptos Narrow"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
     <font>
@@ -776,137 +785,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -927,8 +936,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1465,8 +1480,8 @@
   <sheetPr/>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="113" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -1616,72 +1631,82 @@
       <c r="A13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8" t="s">
-        <v>15</v>
+      <c r="B13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G13" s="2"/>
     </row>
     <row r="14" ht="27.6" spans="1:7">
       <c r="A14" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G14" s="2"/>
     </row>
     <row r="15" ht="30" customHeight="1" spans="1:7">
       <c r="A15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G15" s="2"/>
     </row>
     <row r="16" ht="34" customHeight="1" spans="1:7">
       <c r="A16" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>15</v>
+      <c r="C16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" ht="27.6" spans="1:7">
+    <row r="17" spans="1:7">
       <c r="A17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G17" s="2"/>
     </row>
     <row r="18" ht="27" customHeight="1" spans="1:7">
       <c r="A18" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1692,395 +1717,455 @@
     </row>
     <row r="19" ht="18" customHeight="1" spans="1:7">
       <c r="A19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8" t="s">
-        <v>15</v>
+        <v>23</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G19" s="2"/>
     </row>
     <row r="20" ht="45" customHeight="1" spans="1:7">
       <c r="A20" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8" t="s">
-        <v>15</v>
+        <v>24</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G20" s="2"/>
     </row>
     <row r="21" ht="16" customHeight="1" spans="1:7">
       <c r="A21" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8" t="s">
-        <v>15</v>
+        <v>25</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G21" s="2"/>
     </row>
     <row r="22" ht="23" customHeight="1" spans="1:7">
       <c r="A22" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G23" s="2"/>
     </row>
     <row r="24" ht="50" customHeight="1" spans="1:7">
       <c r="A24" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>15</v>
+      <c r="B24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8" t="s">
-        <v>15</v>
+        <v>30</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G25" s="2"/>
     </row>
     <row r="26" ht="25" customHeight="1" spans="1:7">
       <c r="A26" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8" t="s">
-        <v>15</v>
+        <v>31</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G26" s="2"/>
     </row>
     <row r="27" ht="18" customHeight="1" spans="1:7">
       <c r="A27" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8" t="s">
-        <v>15</v>
+        <v>32</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G27" s="2"/>
     </row>
     <row r="28" ht="18" customHeight="1" spans="1:7">
       <c r="A28" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8" t="s">
-        <v>15</v>
+        <v>33</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G28" s="2"/>
     </row>
     <row r="29" ht="31" customHeight="1" spans="1:7">
       <c r="A29" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8" t="s">
-        <v>15</v>
+        <v>34</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G29" s="2"/>
     </row>
     <row r="30" ht="16" customHeight="1" spans="1:7">
       <c r="A30" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8" t="s">
-        <v>15</v>
+        <v>35</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8" t="s">
-        <v>15</v>
+        <v>36</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G31" s="2"/>
     </row>
     <row r="32" ht="20" customHeight="1" spans="1:7">
       <c r="A32" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8" t="s">
-        <v>15</v>
+        <v>37</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8" t="s">
-        <v>15</v>
+        <v>38</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G33" s="2"/>
     </row>
     <row r="34" ht="20" customHeight="1" spans="1:7">
       <c r="A34" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8" t="s">
-        <v>15</v>
+        <v>39</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8" t="s">
-        <v>15</v>
+        <v>40</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G35" s="2"/>
     </row>
     <row r="36" ht="18" customHeight="1" spans="1:7">
       <c r="A36" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8" t="s">
-        <v>15</v>
+        <v>41</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8" t="s">
-        <v>15</v>
+        <v>42</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G37" s="2"/>
     </row>
     <row r="38" ht="20" customHeight="1" spans="1:7">
       <c r="A38" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8" t="s">
-        <v>15</v>
+        <v>43</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G39" s="2"/>
     </row>
     <row r="40" ht="17" customHeight="1" spans="1:7">
       <c r="A40" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8" t="s">
-        <v>15</v>
+        <v>45</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G40" s="2"/>
     </row>
     <row r="41" ht="17" customHeight="1" spans="1:7">
       <c r="A41" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8" t="s">
-        <v>15</v>
+        <v>46</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G41" s="2"/>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F42" s="8" t="s">
-        <v>15</v>
+      <c r="B42" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G42" s="2"/>
     </row>
     <row r="43" ht="19" customHeight="1" spans="1:7">
       <c r="A43" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8" t="s">
-        <v>15</v>
+        <v>49</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G43" s="2"/>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8" t="s">
-        <v>15</v>
+        <v>50</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G44" s="2"/>
     </row>
     <row r="45" ht="18" customHeight="1" spans="1:7">
       <c r="A45" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8" t="s">
-        <v>15</v>
+        <v>51</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G45" s="2"/>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8" t="s">
-        <v>15</v>
+        <v>52</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G46" s="2"/>
     </row>
     <row r="47" ht="19" customHeight="1" spans="1:7">
       <c r="A47" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8" t="s">
-        <v>15</v>
+        <v>53</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8" t="s">
-        <v>15</v>
+        <v>54</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G48" s="2"/>
     </row>

</xml_diff>